<commit_message>
Moved drill holes to correct position
</commit_message>
<xml_diff>
--- a/Hardware/standalone/bom.xlsx
+++ b/Hardware/standalone/bom.xlsx
@@ -1003,8 +1003,8 @@
   </sheetPr>
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="L54" sqref="A1:L54"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1217,14 +1217,14 @@
         <v>104</v>
       </c>
       <c r="H6">
-        <v>1669967</v>
+        <v>1192513</v>
       </c>
       <c r="K6" s="7">
-        <v>0.16200000000000001</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="L6" s="7">
         <f>Table1[[#This Row],[Price (For Quantity 100)]]*Table1[[#This Row],[Qty]]</f>
-        <v>0.16200000000000001</v>
+        <v>0.19800000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2637,7 +2637,7 @@
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L54" s="8">
         <f>SUM(Table1[Total Cost])</f>
-        <v>12.661999999999997</v>
+        <v>12.697999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>